<commit_message>
Minor edits to Asmita training pack, CoastalTools manual and grid classes Add beta version of wave ray model
git-svn-id: svn://192.168.0.80/muiApps/Trunk/Asmita@136 5305ae0c-0cd9-424f-b575-fb45b188e99a
</commit_message>
<xml_diff>
--- a/Training exercise/Training exercise-Southampton/SW4e model parameters.xlsx
+++ b/Training exercise/Training exercise-Southampton/SW4e model parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab Code\MUImodels\muiApps\Asmita\Training exercise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab Code\MUImodels\muiApps\Asmita\Training exercise\Training exercise-Southampton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDEA1F5-5893-48CA-A7CA-5DC9507F5D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7771F3D-C88F-482F-B9C4-125EB5871438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24630" yWindow="880" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8840" yWindow="5160" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="105">
   <si>
     <t>concentration imported by advection (kg/m^3)</t>
   </si>
@@ -343,6 +343,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>volume increase</t>
+  </si>
+  <si>
+    <t>due to slr over 200 years</t>
   </si>
 </sst>
 </file>
@@ -495,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -747,18 +753,15 @@
     <xf numFmtId="2" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1108,12 +1111,12 @@
   </sheetPr>
   <dimension ref="A1:Q75"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C67" sqref="C67"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1199,10 +1202,12 @@
       <c r="E4" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="103" t="s">
+      <c r="F4" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="16" t="s">
+        <v>103</v>
+      </c>
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
       <c r="J4" s="16"/>
@@ -1213,7 +1218,7 @@
       <c r="O4" s="22"/>
       <c r="P4" s="22"/>
     </row>
-    <row r="5" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A5" s="46" t="s">
         <v>29</v>
       </c>
@@ -1233,7 +1238,9 @@
         <f>SUM(B5:E5)</f>
         <v>61685324</v>
       </c>
-      <c r="G5" s="30"/>
+      <c r="G5" s="30" t="s">
+        <v>104</v>
+      </c>
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
@@ -1264,7 +1271,10 @@
         <f>SUM(B6:E6)</f>
         <v>34383335</v>
       </c>
-      <c r="G6" s="30"/>
+      <c r="G6" s="30">
+        <f>F6*0.002*200</f>
+        <v>13753334</v>
+      </c>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
       <c r="J6" s="30"/>
@@ -1472,16 +1482,16 @@
       <c r="A14" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="102">
+      <c r="B14" s="100">
         <v>0.05</v>
       </c>
-      <c r="C14" s="102">
+      <c r="C14" s="100">
         <v>0.08</v>
       </c>
-      <c r="D14" s="102">
+      <c r="D14" s="100">
         <v>0.05</v>
       </c>
-      <c r="E14" s="102">
+      <c r="E14" s="100">
         <v>0.08</v>
       </c>
       <c r="F14" s="33"/>
@@ -1500,16 +1510,16 @@
       <c r="A15" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="102">
+      <c r="B15" s="100">
         <v>1.23</v>
       </c>
-      <c r="C15" s="102">
+      <c r="C15" s="100">
         <v>1.08</v>
       </c>
-      <c r="D15" s="102">
+      <c r="D15" s="100">
         <v>1.23</v>
       </c>
-      <c r="E15" s="102">
+      <c r="E15" s="100">
         <v>1.08</v>
       </c>
       <c r="F15" s="34"/>
@@ -2248,7 +2258,7 @@
       <c r="A57" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="B57" s="101">
+      <c r="B57" s="32">
         <v>2E-3</v>
       </c>
       <c r="C57" s="49"/>
@@ -2418,7 +2428,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
@@ -2472,22 +2482,22 @@
       <c r="A3" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="102" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100" t="s">
+      <c r="C3" s="102"/>
+      <c r="D3" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100" t="s">
+      <c r="E3" s="102"/>
+      <c r="F3" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100" t="s">
+      <c r="G3" s="102"/>
+      <c r="H3" s="102" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="100"/>
+      <c r="I3" s="102"/>
     </row>
     <row r="4" spans="1:22" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="95"/>

</xml_diff>

<commit_message>
Added functions to allow Asmita to be run from the command line in silent mode (no UI) Added unit testing folder with functions and data for range of tests Updated manual Added option to plot centre-line to ChannelForm model
git-svn-id: svn://192.168.0.80/muiApps/Trunk/Asmita@167 5305ae0c-0cd9-424f-b575-fb45b188e99a
</commit_message>
<xml_diff>
--- a/Training exercise/Training exercise-Southampton/SW4e model parameters.xlsx
+++ b/Training exercise/Training exercise-Southampton/SW4e model parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab Code\MUImodels\muiApps\Asmita\Training exercise\Training exercise-Southampton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7771F3D-C88F-482F-B9C4-125EB5871438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A65020-6BF3-43DD-99E6-7728CC36AE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8840" yWindow="5160" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14290" yWindow="6980" windowWidth="21940" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="106">
   <si>
     <t>concentration imported by advection (kg/m^3)</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>due to slr over 200 years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">effective width </t>
   </si>
 </sst>
 </file>
@@ -633,9 +636,6 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -761,6 +761,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1112,11 +1115,11 @@
   <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1202,7 +1205,7 @@
       <c r="E4" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="101" t="s">
+      <c r="F4" s="100" t="s">
         <v>102</v>
       </c>
       <c r="G4" s="16" t="s">
@@ -1289,16 +1292,16 @@
       <c r="A7" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="75">
+      <c r="B7" s="74">
         <v>4</v>
       </c>
-      <c r="C7" s="75">
+      <c r="C7" s="74">
         <v>4</v>
       </c>
-      <c r="D7" s="75">
+      <c r="D7" s="74">
         <v>4</v>
       </c>
-      <c r="E7" s="75">
+      <c r="E7" s="74">
         <v>4</v>
       </c>
       <c r="F7" s="30"/>
@@ -1317,16 +1320,16 @@
       <c r="A8" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="76">
+      <c r="B8" s="75">
         <v>10000</v>
       </c>
-      <c r="C8" s="76">
+      <c r="C8" s="75">
         <v>10000</v>
       </c>
-      <c r="D8" s="76">
+      <c r="D8" s="75">
         <v>8000</v>
       </c>
-      <c r="E8" s="76">
+      <c r="E8" s="75">
         <v>8000</v>
       </c>
       <c r="F8" s="30"/>
@@ -1341,8 +1344,8 @@
       <c r="O8" s="31"/>
       <c r="P8" s="31"/>
     </row>
-    <row r="9" spans="1:16" s="69" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="66" t="s">
+    <row r="9" spans="1:16" s="68" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="65" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="48">
@@ -1357,17 +1360,17 @@
       <c r="E9" s="48">
         <v>2</v>
       </c>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="68"/>
-      <c r="O9" s="68"/>
-      <c r="P9" s="68"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="67"/>
+      <c r="O9" s="67"/>
+      <c r="P9" s="67"/>
     </row>
     <row r="10" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="46" t="s">
@@ -1398,8 +1401,8 @@
       <c r="O10" s="31"/>
       <c r="P10" s="31"/>
     </row>
-    <row r="11" spans="1:16" s="69" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="70" t="s">
+    <row r="11" spans="1:16" s="68" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="69" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="17">
@@ -1414,20 +1417,20 @@
       <c r="E11" s="17">
         <v>1350</v>
       </c>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="67"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="68"/>
-      <c r="O11" s="68"/>
-      <c r="P11" s="68"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="67"/>
+      <c r="P11" s="67"/>
     </row>
     <row r="12" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="71" t="s">
+      <c r="A12" s="70" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="36">
@@ -1442,14 +1445,14 @@
       <c r="E12" s="36">
         <v>5</v>
       </c>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="72"/>
-      <c r="K12" s="72"/>
-      <c r="L12" s="72"/>
-      <c r="M12" s="72"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="71"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="46" t="s">
@@ -1482,16 +1485,16 @@
       <c r="A14" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="100">
+      <c r="B14" s="99">
         <v>0.05</v>
       </c>
-      <c r="C14" s="100">
+      <c r="C14" s="99">
         <v>0.08</v>
       </c>
-      <c r="D14" s="100">
+      <c r="D14" s="99">
         <v>0.05</v>
       </c>
-      <c r="E14" s="100">
+      <c r="E14" s="99">
         <v>0.08</v>
       </c>
       <c r="F14" s="33"/>
@@ -1510,16 +1513,16 @@
       <c r="A15" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="100">
+      <c r="B15" s="99">
         <v>1.23</v>
       </c>
-      <c r="C15" s="100">
+      <c r="C15" s="99">
         <v>1.08</v>
       </c>
-      <c r="D15" s="100">
+      <c r="D15" s="99">
         <v>1.23</v>
       </c>
-      <c r="E15" s="100">
+      <c r="E15" s="99">
         <v>1.08</v>
       </c>
       <c r="F15" s="34"/>
@@ -1534,29 +1537,29 @@
       <c r="O15"/>
     </row>
     <row r="16" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="71" t="s">
+      <c r="A16" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="73">
-        <v>0</v>
-      </c>
-      <c r="C16" s="73">
-        <v>0</v>
-      </c>
-      <c r="D16" s="73">
-        <v>0</v>
-      </c>
-      <c r="E16" s="73">
-        <v>0</v>
-      </c>
-      <c r="F16" s="74"/>
-      <c r="G16" s="71"/>
-      <c r="H16" s="74"/>
-      <c r="I16" s="74"/>
-      <c r="J16" s="74"/>
-      <c r="K16" s="74"/>
-      <c r="L16" s="74"/>
-      <c r="M16" s="74"/>
+      <c r="B16" s="72">
+        <v>0</v>
+      </c>
+      <c r="C16" s="72">
+        <v>0</v>
+      </c>
+      <c r="D16" s="72">
+        <v>0</v>
+      </c>
+      <c r="E16" s="72">
+        <v>0</v>
+      </c>
+      <c r="F16" s="73"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="73"/>
+      <c r="L16" s="73"/>
+      <c r="M16" s="73"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
@@ -1646,7 +1649,7 @@
       <c r="O19"/>
     </row>
     <row r="20" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="65" t="s">
+      <c r="A20" s="64" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="39">
@@ -1675,20 +1678,20 @@
       <c r="M20" s="39"/>
     </row>
     <row r="21" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="65" t="s">
+      <c r="A21" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="77" t="s">
+      <c r="B21" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="78">
+      <c r="C21" s="77">
         <f>C6/C8/C9</f>
         <v>404.93865</v>
       </c>
-      <c r="D21" s="77" t="s">
+      <c r="D21" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="78">
+      <c r="E21" s="77">
         <f>E6/E8/E9</f>
         <v>312.25968749999998</v>
       </c>
@@ -1702,7 +1705,7 @@
       <c r="M21" s="41"/>
     </row>
     <row r="22" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="65" t="s">
+      <c r="A22" s="64" t="s">
         <v>43</v>
       </c>
       <c r="B22" s="42">
@@ -1731,7 +1734,7 @@
       <c r="M22" s="42"/>
     </row>
     <row r="23" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="65" t="s">
+      <c r="A23" s="64" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="42">
@@ -1759,50 +1762,50 @@
       <c r="L23" s="42"/>
       <c r="M23" s="42"/>
     </row>
-    <row r="24" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="79" t="s">
+    <row r="24" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="80">
+      <c r="B24" s="79">
         <f>B22*B17/B23</f>
         <v>1316.7761897767923</v>
       </c>
-      <c r="C24" s="80">
+      <c r="C24" s="79">
         <f>C22*C17/C23</f>
         <v>1316.7761897767923</v>
       </c>
-      <c r="D24" s="80">
+      <c r="D24" s="79">
         <f>D22*D17/D23</f>
         <v>140.8396434046474</v>
       </c>
-      <c r="E24" s="80">
+      <c r="E24" s="79">
         <f>E22*E17/E23</f>
         <v>140.8396434046474</v>
       </c>
-      <c r="F24" s="80"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="80"/>
-      <c r="I24" s="80"/>
-      <c r="J24" s="80"/>
-      <c r="K24" s="80"/>
-      <c r="L24" s="80"/>
-      <c r="M24" s="80"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="79"/>
     </row>
     <row r="25" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="65" t="s">
+      <c r="A25" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="77" t="s">
+      <c r="B25" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="78">
+      <c r="C25" s="77">
         <f>C22*C7/2*C8/C23</f>
         <v>1572.2700773454237</v>
       </c>
-      <c r="D25" s="77" t="s">
+      <c r="D25" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="78">
+      <c r="E25" s="77">
         <f>E22*E7/2*E8/E23</f>
         <v>395.33934990778221</v>
       </c>
@@ -1816,20 +1819,20 @@
       <c r="M25" s="42"/>
     </row>
     <row r="26" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="65" t="s">
+      <c r="A26" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="77" t="s">
+      <c r="B26" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="78">
+      <c r="C26" s="77">
         <f>C19^2*C20/C13*C7/2*C8/C23</f>
         <v>1481.1522878628059</v>
       </c>
-      <c r="D26" s="77" t="s">
+      <c r="D26" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="78">
+      <c r="E26" s="77">
         <f>E19^2*E20/E13*E7/2*E8/E23</f>
         <v>193.96847063619333</v>
       </c>
@@ -1843,7 +1846,7 @@
       <c r="M26" s="42"/>
     </row>
     <row r="27" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="65" t="s">
+      <c r="A27" s="64" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="40" t="s">
@@ -1870,7 +1873,7 @@
       <c r="M27" s="44"/>
     </row>
     <row r="28" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="65" t="s">
+      <c r="A28" s="64" t="s">
         <v>49</v>
       </c>
       <c r="B28" s="40" t="s">
@@ -1896,32 +1899,32 @@
       <c r="L28" s="44"/>
       <c r="M28" s="44"/>
     </row>
-    <row r="29" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="79" t="s">
+    <row r="29" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="81" t="s">
+      <c r="B29" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="82">
+      <c r="C29" s="81">
         <f>C28*C7/2*C8/C21</f>
         <v>76.745327137221338</v>
       </c>
-      <c r="D29" s="81" t="s">
+      <c r="D29" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="E29" s="82">
+      <c r="E29" s="81">
         <f>E28*E7/2*E8/E21</f>
         <v>28.417213490722222</v>
       </c>
-      <c r="F29" s="83"/>
-      <c r="G29" s="83"/>
-      <c r="H29" s="84"/>
-      <c r="I29" s="84"/>
-      <c r="J29" s="83"/>
-      <c r="K29" s="83"/>
-      <c r="L29" s="84"/>
-      <c r="M29" s="84"/>
+      <c r="F29" s="82"/>
+      <c r="G29" s="82"/>
+      <c r="H29" s="83"/>
+      <c r="I29" s="83"/>
+      <c r="J29" s="82"/>
+      <c r="K29" s="82"/>
+      <c r="L29" s="83"/>
+      <c r="M29" s="83"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B30" s="8"/>
@@ -2016,203 +2019,218 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A43" s="52"/>
-      <c r="B43" s="51"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="51"/>
-    </row>
-    <row r="44" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="53" t="s">
+      <c r="A43" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43" s="102">
+        <f>B6/B8</f>
+        <v>1617.3938000000001</v>
+      </c>
+      <c r="C43" s="102">
+        <f t="shared" ref="C43:E43" si="0">C6/C8</f>
+        <v>809.87729999999999</v>
+      </c>
+      <c r="D43" s="102">
+        <f t="shared" si="0"/>
+        <v>639.30862500000001</v>
+      </c>
+      <c r="E43" s="102">
+        <f t="shared" si="0"/>
+        <v>624.51937499999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B44" s="54" t="s">
+      <c r="B44" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="C44" s="55" t="s">
+      <c r="C44" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="55" t="s">
+      <c r="D44" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="E44" s="55"/>
-      <c r="F44" s="56"/>
-      <c r="G44" s="56"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="56"/>
-      <c r="J44" s="56"/>
-      <c r="K44" s="56"/>
-      <c r="L44" s="57"/>
-      <c r="M44" s="58"/>
-      <c r="N44" s="58"/>
-      <c r="O44" s="58"/>
-    </row>
-    <row r="45" spans="1:17" s="59" customFormat="1" ht="87.5" x14ac:dyDescent="0.3">
-      <c r="A45" s="99" t="s">
+      <c r="E44" s="54"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="55"/>
+      <c r="H44" s="55"/>
+      <c r="I44" s="55"/>
+      <c r="J44" s="55"/>
+      <c r="K44" s="55"/>
+      <c r="L44" s="56"/>
+      <c r="M44" s="57"/>
+      <c r="N44" s="57"/>
+      <c r="O44" s="57"/>
+    </row>
+    <row r="45" spans="1:17" s="58" customFormat="1" ht="87.5" x14ac:dyDescent="0.3">
+      <c r="A45" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="61" t="s">
+      <c r="B45" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="C45" s="61" t="s">
+      <c r="C45" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="61" t="s">
+      <c r="D45" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="61"/>
-      <c r="F45" s="57"/>
-      <c r="G45" s="57"/>
-      <c r="H45" s="57"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
-      <c r="K45" s="56"/>
-      <c r="L45" s="57"/>
-      <c r="M45" s="58"/>
-      <c r="N45" s="58"/>
-      <c r="O45" s="58"/>
-    </row>
-    <row r="46" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="62" t="s">
+      <c r="E45" s="60"/>
+      <c r="F45" s="56"/>
+      <c r="G45" s="56"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="55"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="55"/>
+      <c r="L45" s="56"/>
+      <c r="M45" s="57"/>
+      <c r="N45" s="57"/>
+      <c r="O45" s="57"/>
+    </row>
+    <row r="46" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="63" t="s">
+      <c r="B46" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="60"/>
-      <c r="D46" s="57"/>
-      <c r="E46" s="57"/>
-      <c r="F46" s="57"/>
-      <c r="G46" s="57"/>
-      <c r="H46" s="57"/>
-      <c r="I46" s="64"/>
-      <c r="J46" s="57"/>
-      <c r="L46" s="57"/>
-      <c r="M46" s="58"/>
-      <c r="N46" s="58"/>
-      <c r="O46" s="58"/>
-    </row>
-    <row r="47" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="62" t="s">
+      <c r="C46" s="59"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="56"/>
+      <c r="G46" s="56"/>
+      <c r="H46" s="56"/>
+      <c r="I46" s="63"/>
+      <c r="J46" s="56"/>
+      <c r="L46" s="56"/>
+      <c r="M46" s="57"/>
+      <c r="N46" s="57"/>
+      <c r="O46" s="57"/>
+    </row>
+    <row r="47" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="63" t="s">
+      <c r="B47" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="60"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="57"/>
-      <c r="F47" s="57"/>
-      <c r="G47" s="57"/>
-      <c r="H47" s="57"/>
-      <c r="I47" s="64"/>
-      <c r="J47" s="64"/>
-      <c r="K47" s="57"/>
-      <c r="L47" s="57"/>
-      <c r="M47" s="58"/>
-      <c r="N47" s="58"/>
-      <c r="O47" s="58"/>
-    </row>
-    <row r="48" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="62" t="s">
+      <c r="C47" s="59"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="56"/>
+      <c r="G47" s="56"/>
+      <c r="H47" s="56"/>
+      <c r="I47" s="63"/>
+      <c r="J47" s="63"/>
+      <c r="K47" s="56"/>
+      <c r="L47" s="56"/>
+      <c r="M47" s="57"/>
+      <c r="N47" s="57"/>
+      <c r="O47" s="57"/>
+    </row>
+    <row r="48" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="B48" s="63" t="s">
+      <c r="B48" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="60"/>
-      <c r="D48" s="57"/>
-      <c r="E48" s="57"/>
-      <c r="F48" s="57"/>
-      <c r="G48" s="57"/>
-      <c r="H48" s="57"/>
-      <c r="I48" s="64"/>
-      <c r="J48" s="64"/>
-      <c r="L48" s="57"/>
-      <c r="M48" s="58"/>
-      <c r="N48" s="58"/>
-      <c r="O48" s="58"/>
-    </row>
-    <row r="49" spans="1:15" s="59" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="62" t="s">
+      <c r="C48" s="59"/>
+      <c r="D48" s="56"/>
+      <c r="E48" s="56"/>
+      <c r="F48" s="56"/>
+      <c r="G48" s="56"/>
+      <c r="H48" s="56"/>
+      <c r="I48" s="63"/>
+      <c r="J48" s="63"/>
+      <c r="L48" s="56"/>
+      <c r="M48" s="57"/>
+      <c r="N48" s="57"/>
+      <c r="O48" s="57"/>
+    </row>
+    <row r="49" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="63" t="s">
+      <c r="B49" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="60"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="57"/>
-      <c r="F49" s="57"/>
-      <c r="G49" s="57"/>
-      <c r="H49" s="57"/>
-      <c r="I49" s="64"/>
-      <c r="J49" s="64"/>
-      <c r="L49" s="57"/>
-      <c r="M49" s="58"/>
-      <c r="N49" s="58"/>
-      <c r="O49" s="58"/>
-    </row>
-    <row r="50" spans="1:15" s="59" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="62" t="s">
+      <c r="C49" s="59"/>
+      <c r="D49" s="56"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="56"/>
+      <c r="G49" s="56"/>
+      <c r="H49" s="56"/>
+      <c r="I49" s="63"/>
+      <c r="J49" s="63"/>
+      <c r="L49" s="56"/>
+      <c r="M49" s="57"/>
+      <c r="N49" s="57"/>
+      <c r="O49" s="57"/>
+    </row>
+    <row r="50" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="63" t="s">
+      <c r="B50" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="60"/>
-      <c r="D50" s="57"/>
-      <c r="E50" s="57"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="57"/>
-      <c r="H50" s="57"/>
-      <c r="I50" s="64"/>
-      <c r="J50" s="64"/>
-      <c r="L50" s="57"/>
-      <c r="M50" s="58"/>
-      <c r="N50" s="58"/>
-      <c r="O50" s="58"/>
-    </row>
-    <row r="51" spans="1:15" s="59" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="62" t="s">
+      <c r="C50" s="59"/>
+      <c r="D50" s="56"/>
+      <c r="E50" s="56"/>
+      <c r="F50" s="56"/>
+      <c r="G50" s="56"/>
+      <c r="H50" s="56"/>
+      <c r="I50" s="63"/>
+      <c r="J50" s="63"/>
+      <c r="L50" s="56"/>
+      <c r="M50" s="57"/>
+      <c r="N50" s="57"/>
+      <c r="O50" s="57"/>
+    </row>
+    <row r="51" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="B51" s="63" t="s">
+      <c r="B51" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="60"/>
-      <c r="D51" s="57"/>
-      <c r="E51" s="57"/>
-      <c r="F51" s="57"/>
-      <c r="G51" s="57"/>
-      <c r="H51" s="57"/>
-      <c r="I51" s="57"/>
-      <c r="J51" s="57"/>
-      <c r="K51" s="57"/>
-      <c r="L51" s="57"/>
-      <c r="M51" s="58"/>
-      <c r="N51" s="58"/>
-      <c r="O51" s="58"/>
-    </row>
-    <row r="52" spans="1:15" s="59" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="62" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="63" t="s">
+      <c r="C51" s="59"/>
+      <c r="D51" s="56"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="56"/>
+      <c r="H51" s="56"/>
+      <c r="I51" s="56"/>
+      <c r="J51" s="56"/>
+      <c r="K51" s="56"/>
+      <c r="L51" s="56"/>
+      <c r="M51" s="57"/>
+      <c r="N51" s="57"/>
+      <c r="O51" s="57"/>
+    </row>
+    <row r="52" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="C52" s="60"/>
-      <c r="D52" s="57"/>
-      <c r="E52" s="57"/>
-      <c r="F52" s="64"/>
-      <c r="G52" s="64"/>
-      <c r="H52" s="64"/>
-      <c r="I52" s="64"/>
-      <c r="J52" s="64"/>
-      <c r="K52" s="64"/>
-      <c r="L52" s="57"/>
-      <c r="M52" s="58"/>
-      <c r="N52" s="58"/>
-      <c r="O52" s="58"/>
+      <c r="C52" s="59"/>
+      <c r="D52" s="56"/>
+      <c r="E52" s="56"/>
+      <c r="F52" s="63"/>
+      <c r="G52" s="63"/>
+      <c r="H52" s="63"/>
+      <c r="I52" s="63"/>
+      <c r="J52" s="63"/>
+      <c r="K52" s="63"/>
+      <c r="L52" s="56"/>
+      <c r="M52" s="57"/>
+      <c r="N52" s="57"/>
+      <c r="O52" s="57"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F53" s="20"/>
@@ -2223,10 +2241,10 @@
       <c r="K53" s="20"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A54" s="65" t="s">
+      <c r="A54" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="B54" s="65"/>
+      <c r="B54" s="64"/>
       <c r="C54" s="49"/>
       <c r="F54" s="21"/>
       <c r="G54" s="21"/>
@@ -2276,7 +2294,7 @@
       <c r="A59" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="B59" s="98">
+      <c r="B59" s="97">
         <v>0.15</v>
       </c>
       <c r="C59" s="49"/>
@@ -2285,7 +2303,7 @@
       <c r="A60" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="B60" s="98">
+      <c r="B60" s="97">
         <v>18.600000000000001</v>
       </c>
       <c r="C60" s="49"/>
@@ -2294,7 +2312,7 @@
       <c r="A61" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="B61" s="98">
+      <c r="B61" s="97">
         <v>12.2</v>
       </c>
       <c r="C61" s="49"/>
@@ -2309,10 +2327,10 @@
       <c r="C62" s="49"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A63" s="65" t="s">
+      <c r="A63" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="B63" s="65"/>
+      <c r="B63" s="64"/>
       <c r="C63" s="49"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
@@ -2361,10 +2379,10 @@
       <c r="C68" s="49"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="65" t="s">
+      <c r="A69" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="B69" s="65"/>
+      <c r="B69" s="64"/>
       <c r="C69" s="49"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -2394,10 +2412,10 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="65" t="s">
+      <c r="A73" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="B73" s="65"/>
+      <c r="B73" s="64"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="46" t="s">
@@ -2435,14 +2453,14 @@
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.08984375" style="18" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" style="88" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" style="91" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" style="88" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" style="91" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" style="88" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" style="91" customWidth="1"/>
-    <col min="8" max="8" width="12.7265625" style="88" customWidth="1"/>
-    <col min="9" max="9" width="12.7265625" style="91" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" style="87" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" style="90" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" style="87" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" style="90" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" style="87" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" style="90" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" style="87" customWidth="1"/>
+    <col min="9" max="9" width="12.7265625" style="90" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
@@ -2453,7 +2471,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="91" t="s">
         <v>51</v>
       </c>
       <c r="B1" s="19"/>
@@ -2466,7 +2484,7 @@
       <c r="I1"/>
     </row>
     <row r="2" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="92" t="s">
         <v>61</v>
       </c>
       <c r="B2" s="19"/>
@@ -2478,175 +2496,175 @@
       <c r="H2" s="19"/>
       <c r="I2"/>
     </row>
-    <row r="3" spans="1:22" s="86" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="85" t="s">
+    <row r="3" spans="1:22" s="85" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A3" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="101" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102" t="s">
+      <c r="C3" s="101"/>
+      <c r="D3" s="101" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102" t="s">
+      <c r="E3" s="101"/>
+      <c r="F3" s="101" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102" t="s">
+      <c r="G3" s="101"/>
+      <c r="H3" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="102"/>
-    </row>
-    <row r="4" spans="1:22" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="95"/>
-      <c r="B4" s="89" t="s">
+      <c r="I3" s="101"/>
+    </row>
+    <row r="4" spans="1:22" s="85" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="94"/>
+      <c r="B4" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="89" t="s">
+      <c r="D4" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="89" t="s">
+      <c r="E4" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="89" t="s">
+      <c r="F4" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="89" t="s">
+      <c r="G4" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="89" t="s">
+      <c r="H4" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="89" t="s">
+      <c r="I4" s="88" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="94" t="s">
+    <row r="5" spans="1:22" s="85" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="89" t="s">
+      <c r="C5" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="89" t="s">
+      <c r="D5" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="89" t="s">
+      <c r="E5" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="89" t="s">
+      <c r="F5" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="89" t="s">
+      <c r="G5" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="89" t="s">
+      <c r="H5" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="89" t="s">
+      <c r="I5" s="88" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="94">
+      <c r="A6" s="93">
         <v>1926</v>
       </c>
-      <c r="B6" s="87"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="87">
-        <v>0</v>
-      </c>
-      <c r="E6" s="90"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="88">
+      <c r="B6" s="86"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="86">
+        <v>0</v>
+      </c>
+      <c r="E6" s="89"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="87">
         <v>420000</v>
       </c>
-      <c r="I6" s="91">
+      <c r="I6" s="90">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A7" s="94">
+      <c r="A7" s="93">
         <v>1927</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="96">
+      <c r="B7" s="86"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="95">
         <v>420000</v>
       </c>
-      <c r="F7" s="87"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="88">
+      <c r="F7" s="86"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="87">
         <v>-2098785</v>
       </c>
-      <c r="I7" s="91">
+      <c r="I7" s="90">
         <v>-667500</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A8" s="94">
+      <c r="A8" s="93">
         <v>1928</v>
       </c>
-      <c r="B8" s="87"/>
-      <c r="C8" s="90"/>
-      <c r="D8" s="96">
+      <c r="B8" s="86"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="95">
         <v>420000</v>
       </c>
-      <c r="F8" s="87"/>
-      <c r="G8" s="90"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="89"/>
     </row>
     <row r="9" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A9" s="94">
+      <c r="A9" s="93">
         <v>1929</v>
       </c>
-      <c r="B9" s="87"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="96">
+      <c r="B9" s="86"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="95">
         <v>420000</v>
       </c>
-      <c r="F9" s="87"/>
-      <c r="G9" s="90"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="89"/>
     </row>
     <row r="10" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="94">
+      <c r="A10" s="93">
         <v>1930</v>
       </c>
-      <c r="D10" s="96">
+      <c r="D10" s="95">
         <v>420000</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="94">
+      <c r="A11" s="93">
         <v>1931</v>
       </c>
-      <c r="D11" s="88">
+      <c r="D11" s="87">
         <v>965050</v>
       </c>
-      <c r="E11" s="91">
+      <c r="E11" s="90">
         <v>710743</v>
       </c>
-      <c r="H11" s="88">
+      <c r="H11" s="87">
         <v>-2305143</v>
       </c>
-      <c r="I11" s="91">
+      <c r="I11" s="90">
         <v>-1147381</v>
       </c>
       <c r="N11" s="28"/>
     </row>
     <row r="12" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A12" s="94">
+      <c r="A12" s="93">
         <v>1932</v>
       </c>
-      <c r="D12" s="96">
+      <c r="D12" s="95">
         <v>420000</v>
       </c>
       <c r="M12" s="18"/>
@@ -2661,10 +2679,10 @@
       <c r="V12" s="19"/>
     </row>
     <row r="13" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A13" s="94">
+      <c r="A13" s="93">
         <v>1933</v>
       </c>
-      <c r="D13" s="96">
+      <c r="D13" s="95">
         <v>420000</v>
       </c>
       <c r="M13" s="18"/>
@@ -2679,10 +2697,10 @@
       <c r="V13" s="19"/>
     </row>
     <row r="14" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A14" s="94">
+      <c r="A14" s="93">
         <v>1934</v>
       </c>
-      <c r="D14" s="96">
+      <c r="D14" s="95">
         <v>420000</v>
       </c>
       <c r="M14" s="19"/>
@@ -2696,10 +2714,10 @@
       <c r="U14" s="9"/>
     </row>
     <row r="15" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A15" s="94">
+      <c r="A15" s="93">
         <v>1935</v>
       </c>
-      <c r="D15" s="96">
+      <c r="D15" s="95">
         <v>420000</v>
       </c>
       <c r="M15" s="19"/>
@@ -2713,10 +2731,10 @@
       <c r="U15" s="9"/>
     </row>
     <row r="16" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A16" s="94">
+      <c r="A16" s="93">
         <v>1936</v>
       </c>
-      <c r="D16" s="96">
+      <c r="D16" s="95">
         <v>420000</v>
       </c>
       <c r="M16" s="19"/>
@@ -2730,10 +2748,10 @@
       <c r="U16" s="9"/>
     </row>
     <row r="17" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A17" s="94">
+      <c r="A17" s="93">
         <v>1937</v>
       </c>
-      <c r="D17" s="96">
+      <c r="D17" s="95">
         <v>420000</v>
       </c>
       <c r="M17" s="19"/>
@@ -2747,13 +2765,13 @@
       <c r="U17" s="9"/>
     </row>
     <row r="18" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A18" s="94">
+      <c r="A18" s="93">
         <v>1938</v>
       </c>
-      <c r="D18" s="97">
+      <c r="D18" s="96">
         <v>920000</v>
       </c>
-      <c r="E18" s="91">
+      <c r="E18" s="90">
         <v>0</v>
       </c>
       <c r="M18" s="19"/>
@@ -2767,10 +2785,10 @@
       <c r="U18" s="9"/>
     </row>
     <row r="19" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A19" s="94">
+      <c r="A19" s="93">
         <v>1939</v>
       </c>
-      <c r="D19" s="96">
+      <c r="D19" s="95">
         <v>370000</v>
       </c>
       <c r="M19" s="19"/>
@@ -2784,19 +2802,19 @@
       <c r="U19" s="9"/>
     </row>
     <row r="20" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A20" s="94">
+      <c r="A20" s="93">
         <v>1940</v>
       </c>
-      <c r="D20" s="96">
+      <c r="D20" s="95">
         <v>370000</v>
       </c>
       <c r="N20" s="29"/>
     </row>
     <row r="21" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A21" s="94">
+      <c r="A21" s="93">
         <v>1941</v>
       </c>
-      <c r="D21" s="96">
+      <c r="D21" s="95">
         <v>370000</v>
       </c>
       <c r="M21" s="24"/>
@@ -2809,10 +2827,10 @@
       <c r="T21" s="5"/>
     </row>
     <row r="22" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A22" s="94">
+      <c r="A22" s="93">
         <v>1942</v>
       </c>
-      <c r="D22" s="96">
+      <c r="D22" s="95">
         <v>370000</v>
       </c>
       <c r="M22" s="23"/>
@@ -2825,10 +2843,10 @@
       <c r="T22" s="5"/>
     </row>
     <row r="23" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A23" s="94">
+      <c r="A23" s="93">
         <v>1943</v>
       </c>
-      <c r="D23" s="96">
+      <c r="D23" s="95">
         <v>370000</v>
       </c>
       <c r="M23" s="23"/>
@@ -2841,10 +2859,10 @@
       <c r="T23" s="5"/>
     </row>
     <row r="24" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A24" s="94">
+      <c r="A24" s="93">
         <v>1944</v>
       </c>
-      <c r="D24" s="96">
+      <c r="D24" s="95">
         <v>370000</v>
       </c>
       <c r="M24" s="23"/>
@@ -2857,10 +2875,10 @@
       <c r="T24" s="5"/>
     </row>
     <row r="25" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A25" s="94">
+      <c r="A25" s="93">
         <v>1945</v>
       </c>
-      <c r="D25" s="96">
+      <c r="D25" s="95">
         <v>370000</v>
       </c>
       <c r="M25" s="23"/>
@@ -2873,10 +2891,10 @@
       <c r="T25" s="5"/>
     </row>
     <row r="26" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A26" s="94">
+      <c r="A26" s="93">
         <v>1946</v>
       </c>
-      <c r="D26" s="96">
+      <c r="D26" s="95">
         <v>370000</v>
       </c>
       <c r="M26" s="23"/>
@@ -2889,10 +2907,10 @@
       <c r="T26" s="5"/>
     </row>
     <row r="27" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A27" s="94">
+      <c r="A27" s="93">
         <v>1947</v>
       </c>
-      <c r="D27" s="96">
+      <c r="D27" s="95">
         <v>370000</v>
       </c>
       <c r="M27" s="23"/>
@@ -2905,461 +2923,461 @@
       <c r="T27" s="5"/>
     </row>
     <row r="28" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A28" s="94">
+      <c r="A28" s="93">
         <v>1948</v>
       </c>
-      <c r="D28" s="96">
+      <c r="D28" s="95">
         <v>370000</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A29" s="94">
+      <c r="A29" s="93">
         <v>1949</v>
       </c>
-      <c r="D29" s="96">
+      <c r="D29" s="95">
         <v>370000</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A30" s="94">
+      <c r="A30" s="93">
         <v>1950</v>
       </c>
-      <c r="D30" s="96">
+      <c r="D30" s="95">
         <v>270000</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A31" s="94">
+      <c r="A31" s="93">
         <v>1951</v>
       </c>
-      <c r="D31" s="96">
+      <c r="D31" s="95">
         <v>270000</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A32" s="94">
+      <c r="A32" s="93">
         <v>1952</v>
       </c>
-      <c r="D32" s="96">
+      <c r="D32" s="95">
         <v>270000</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A33" s="94">
+      <c r="A33" s="93">
         <v>1953</v>
       </c>
-      <c r="D33" s="96">
+      <c r="D33" s="95">
         <v>270000</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A34" s="94">
+      <c r="A34" s="93">
         <v>1954</v>
       </c>
-      <c r="D34" s="96">
+      <c r="D34" s="95">
         <v>270000</v>
       </c>
       <c r="N34" s="11"/>
     </row>
     <row r="35" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A35" s="94">
+      <c r="A35" s="93">
         <v>1955</v>
       </c>
-      <c r="D35" s="96">
+      <c r="D35" s="95">
         <v>270000</v>
       </c>
       <c r="N35" s="11"/>
     </row>
     <row r="36" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A36" s="94">
+      <c r="A36" s="93">
         <v>1956</v>
       </c>
-      <c r="D36" s="96">
+      <c r="D36" s="95">
         <v>270000</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A37" s="94">
+      <c r="A37" s="93">
         <v>1957</v>
       </c>
-      <c r="D37" s="96">
+      <c r="D37" s="95">
         <v>270000</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A38" s="94">
+      <c r="A38" s="93">
         <v>1958</v>
       </c>
-      <c r="D38" s="96">
+      <c r="D38" s="95">
         <v>270000</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A39" s="94">
+      <c r="A39" s="93">
         <v>1959</v>
       </c>
-      <c r="D39" s="96">
+      <c r="D39" s="95">
         <v>270000</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A40" s="94">
+      <c r="A40" s="93">
         <v>1960</v>
       </c>
-      <c r="D40" s="96">
+      <c r="D40" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A41" s="94">
+      <c r="A41" s="93">
         <v>1961</v>
       </c>
-      <c r="D41" s="96">
-        <v>280000</v>
-      </c>
-      <c r="H41" s="88">
+      <c r="D41" s="95">
+        <v>280000</v>
+      </c>
+      <c r="H41" s="87">
         <v>-1523786</v>
       </c>
-      <c r="I41" s="91">
+      <c r="I41" s="90">
         <v>-412500</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A42" s="94">
+      <c r="A42" s="93">
         <v>1962</v>
       </c>
-      <c r="D42" s="96">
+      <c r="D42" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A43" s="94">
+      <c r="A43" s="93">
         <v>1963</v>
       </c>
-      <c r="D43" s="96">
+      <c r="D43" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A44" s="94">
+      <c r="A44" s="93">
         <v>1964</v>
       </c>
-      <c r="D44" s="96">
+      <c r="D44" s="95">
         <v>300000</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="94">
+      <c r="A45" s="93">
         <v>1965</v>
       </c>
-      <c r="B45" s="88">
+      <c r="B45" s="87">
         <v>44506</v>
       </c>
-      <c r="C45" s="91">
+      <c r="C45" s="90">
         <v>48739</v>
       </c>
-      <c r="D45" s="88">
+      <c r="D45" s="87">
         <v>7636675</v>
       </c>
-      <c r="E45" s="91">
+      <c r="E45" s="90">
         <v>343245</v>
       </c>
-      <c r="F45" s="88">
+      <c r="F45" s="87">
         <v>-2695096</v>
       </c>
-      <c r="G45" s="91">
+      <c r="G45" s="90">
         <v>-1861535</v>
       </c>
-      <c r="H45" s="88">
+      <c r="H45" s="87">
         <v>-2830178</v>
       </c>
-      <c r="I45" s="91">
+      <c r="I45" s="90">
         <v>-1371379</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A46" s="94">
+      <c r="A46" s="93">
         <v>1966</v>
       </c>
-      <c r="D46" s="96">
+      <c r="D46" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A47" s="94">
+      <c r="A47" s="93">
         <v>1967</v>
       </c>
-      <c r="D47" s="96">
+      <c r="D47" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A48" s="94">
+      <c r="A48" s="93">
         <v>1968</v>
       </c>
-      <c r="D48" s="96">
+      <c r="D48" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A49" s="94">
+      <c r="A49" s="93">
         <v>1969</v>
       </c>
-      <c r="D49" s="96">
+      <c r="D49" s="95">
         <v>780000</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A50" s="94">
+      <c r="A50" s="93">
         <v>1970</v>
       </c>
-      <c r="D50" s="96">
+      <c r="D50" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A51" s="94">
+      <c r="A51" s="93">
         <v>1971</v>
       </c>
-      <c r="D51" s="96">
+      <c r="D51" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A52" s="94">
+      <c r="A52" s="93">
         <v>1972</v>
       </c>
-      <c r="D52" s="96">
+      <c r="D52" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A53" s="94">
+      <c r="A53" s="93">
         <v>1973</v>
       </c>
-      <c r="D53" s="96">
+      <c r="D53" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A54" s="94">
+      <c r="A54" s="93">
         <v>1974</v>
       </c>
-      <c r="D54" s="96">
+      <c r="D54" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A55" s="94">
+      <c r="A55" s="93">
         <v>1975</v>
       </c>
-      <c r="D55" s="96">
+      <c r="D55" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A56" s="94">
+      <c r="A56" s="93">
         <v>1976</v>
       </c>
-      <c r="D56" s="96">
+      <c r="D56" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A57" s="94">
+      <c r="A57" s="93">
         <v>1977</v>
       </c>
-      <c r="D57" s="96">
+      <c r="D57" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A58" s="94">
+      <c r="A58" s="93">
         <v>1978</v>
       </c>
-      <c r="D58" s="96">
+      <c r="D58" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A59" s="94">
+      <c r="A59" s="93">
         <v>1979</v>
       </c>
-      <c r="D59" s="96">
+      <c r="D59" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A60" s="94">
+      <c r="A60" s="93">
         <v>1980</v>
       </c>
-      <c r="D60" s="96">
+      <c r="D60" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A61" s="94">
+      <c r="A61" s="93">
         <v>1981</v>
       </c>
-      <c r="D61" s="96">
+      <c r="D61" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A62" s="94">
+      <c r="A62" s="93">
         <v>1982</v>
       </c>
-      <c r="D62" s="96">
+      <c r="D62" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A63" s="94">
+      <c r="A63" s="93">
         <v>1983</v>
       </c>
-      <c r="D63" s="96">
+      <c r="D63" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A64" s="94">
+      <c r="A64" s="93">
         <v>1984</v>
       </c>
-      <c r="D64" s="96">
+      <c r="D64" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A65" s="94">
+      <c r="A65" s="93">
         <v>1985</v>
       </c>
-      <c r="D65" s="96">
+      <c r="D65" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A66" s="94">
+      <c r="A66" s="93">
         <v>1986</v>
       </c>
-      <c r="D66" s="96">
+      <c r="D66" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A67" s="94">
+      <c r="A67" s="93">
         <v>1987</v>
       </c>
-      <c r="D67" s="96">
+      <c r="D67" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A68" s="94">
+      <c r="A68" s="93">
         <v>1988</v>
       </c>
-      <c r="D68" s="96">
+      <c r="D68" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A69" s="94">
+      <c r="A69" s="93">
         <v>1989</v>
       </c>
-      <c r="D69" s="96">
+      <c r="D69" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A70" s="94">
+      <c r="A70" s="93">
         <v>1990</v>
       </c>
-      <c r="D70" s="96">
+      <c r="D70" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A71" s="94">
+      <c r="A71" s="93">
         <v>1991</v>
       </c>
-      <c r="D71" s="96">
+      <c r="D71" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A72" s="94">
+      <c r="A72" s="93">
         <v>1992</v>
       </c>
-      <c r="D72" s="96">
+      <c r="D72" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A73" s="94">
+      <c r="A73" s="93">
         <v>1993</v>
       </c>
-      <c r="D73" s="96">
+      <c r="D73" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A74" s="94">
+      <c r="A74" s="93">
         <v>1994</v>
       </c>
-      <c r="D74" s="96">
+      <c r="D74" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="94">
+      <c r="A75" s="93">
         <v>1995</v>
       </c>
-      <c r="D75" s="88">
+      <c r="D75" s="87">
         <v>3280000</v>
       </c>
-      <c r="E75" s="91">
+      <c r="E75" s="90">
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A76" s="94">
+      <c r="A76" s="93">
         <v>1996</v>
       </c>
-      <c r="D76" s="96">
+      <c r="D76" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A77" s="94">
+      <c r="A77" s="93">
         <v>1997</v>
       </c>
-      <c r="D77" s="96">
+      <c r="D77" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="94">
+      <c r="A78" s="93">
         <v>1998</v>
       </c>
-      <c r="D78" s="88">
+      <c r="D78" s="87">
         <v>2280000</v>
       </c>
-      <c r="E78" s="91">
+      <c r="E78" s="90">
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A79" s="94">
+      <c r="A79" s="93">
         <v>1999</v>
       </c>
-      <c r="D79" s="96">
+      <c r="D79" s="95">
         <v>280000</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A80" s="94">
+      <c r="A80" s="93">
         <v>2000</v>
       </c>
-      <c r="D80" s="96">
+      <c r="D80" s="95">
         <v>280000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified interventions and sorted problems with intertidal in Southampton model (see notes in Book 14)
git-svn-id: svn://192.168.0.80/muiApps/Trunk/Asmita@220 5305ae0c-0cd9-424f-b575-fb45b188e99a
</commit_message>
<xml_diff>
--- a/Training exercise/Training exercise-Southampton/SW4e model parameters.xlsx
+++ b/Training exercise/Training exercise-Southampton/SW4e model parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab Code\MUImodels\muiApps\Asmita\Training exercise\Training exercise-Southampton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab Code\MUImodels\v35Asmita\Training exercise\Training exercise-Southampton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A65020-6BF3-43DD-99E6-7728CC36AE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6307DF0-90DF-4DF0-9C67-43F05E39EFB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14290" yWindow="6980" windowWidth="21940" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,45 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ian Townend</author>
+  </authors>
+  <commentList>
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{23411808-4DC3-431A-9B47-853680B69922}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ian Townend:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Source 
+Table 2
+Rossington S K, Nicholls R J, Stive M J F and Wang Z B, 2011, Estuary schematisation in behaviour-oriented modelling. Marine Geology, 281 (1-4), 27-34, 10.1016/j.margeo.2011.01.005.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="112">
   <si>
     <t>concentration imported by advection (kg/m^3)</t>
   </si>
@@ -352,6 +389,24 @@
   </si>
   <si>
     <t xml:space="preserve">effective width </t>
+  </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>Net</t>
+  </si>
+  <si>
+    <t>Depth0</t>
+  </si>
+  <si>
+    <t>Depth1</t>
+  </si>
+  <si>
+    <t>Calibrated using inner channel maintenance dredge to give no volume change with slr=0</t>
+  </si>
+  <si>
+    <t>Not used</t>
   </si>
 </sst>
 </file>
@@ -365,7 +420,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -441,6 +496,30 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -504,7 +583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -745,7 +824,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -760,10 +838,25 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -789,9 +882,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -829,9 +922,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -864,26 +957,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -916,26 +992,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1108,18 +1167,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1205,7 +1264,7 @@
       <c r="E4" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="100" t="s">
+      <c r="F4" s="99" t="s">
         <v>102</v>
       </c>
       <c r="G4" s="16" t="s">
@@ -1221,7 +1280,7 @@
       <c r="O4" s="22"/>
       <c r="P4" s="22"/>
     </row>
-    <row r="5" spans="1:16" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="46" t="s">
         <v>29</v>
       </c>
@@ -1229,17 +1288,17 @@
         <v>17640829</v>
       </c>
       <c r="C5" s="30">
-        <v>23242981</v>
+        <v>9200000</v>
       </c>
       <c r="D5" s="30">
         <v>12195117</v>
       </c>
       <c r="E5" s="30">
-        <v>8606397</v>
+        <v>11400000</v>
       </c>
       <c r="F5" s="45">
         <f>SUM(B5:E5)</f>
-        <v>61685324</v>
+        <v>50435946</v>
       </c>
       <c r="G5" s="30" t="s">
         <v>104</v>
@@ -1458,17 +1517,17 @@
       <c r="A13" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="34">
+      <c r="B13" s="110">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="C13" s="34">
+      <c r="C13" s="110">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="D13" s="110">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D13" s="34">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="E13" s="34">
-        <v>3.0000000000000001E-3</v>
+      <c r="E13" s="110">
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="F13" s="32"/>
       <c r="G13" s="32"/>
@@ -1485,17 +1544,17 @@
       <c r="A14" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="99">
-        <v>0.05</v>
-      </c>
-      <c r="C14" s="99">
-        <v>0.08</v>
-      </c>
-      <c r="D14" s="99">
-        <v>0.05</v>
-      </c>
-      <c r="E14" s="99">
-        <v>0.08</v>
+      <c r="B14" s="98">
+        <v>1</v>
+      </c>
+      <c r="C14" s="98">
+        <v>1</v>
+      </c>
+      <c r="D14" s="98">
+        <v>1</v>
+      </c>
+      <c r="E14" s="98">
+        <v>1</v>
       </c>
       <c r="F14" s="33"/>
       <c r="G14" s="46"/>
@@ -1513,17 +1572,17 @@
       <c r="A15" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="99">
-        <v>1.23</v>
-      </c>
-      <c r="C15" s="99">
-        <v>1.08</v>
-      </c>
-      <c r="D15" s="99">
-        <v>1.23</v>
-      </c>
-      <c r="E15" s="99">
-        <v>1.08</v>
+      <c r="B15" s="98">
+        <v>1</v>
+      </c>
+      <c r="C15" s="98">
+        <v>1</v>
+      </c>
+      <c r="D15" s="98">
+        <v>1</v>
+      </c>
+      <c r="E15" s="98">
+        <v>1</v>
       </c>
       <c r="F15" s="34"/>
       <c r="G15" s="46"/>
@@ -1596,19 +1655,19 @@
       </c>
       <c r="B18" s="35">
         <f>(B5+(C5+B6*B7)/2)/(B6+C6/2)</f>
-        <v>3.0464919603104823</v>
+        <v>2.699294322256462</v>
       </c>
       <c r="C18" s="35">
         <f>B18</f>
-        <v>3.0464919603104823</v>
+        <v>2.699294322256462</v>
       </c>
       <c r="D18" s="35">
         <f>(D5+(E5+D6*D7)/2)/(D6+E6/2)</f>
-        <v>3.5109478149000468</v>
+        <v>3.6944345758676156</v>
       </c>
       <c r="E18" s="35">
         <f>D18</f>
-        <v>3.5109478149000468</v>
+        <v>3.6944345758676156</v>
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="46"/>
@@ -1626,16 +1685,16 @@
         <v>38</v>
       </c>
       <c r="B19" s="35">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="C19" s="35">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="D19" s="35">
-        <v>0.3</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E19" s="35">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="F19" s="35"/>
       <c r="G19" s="47"/>
@@ -1658,7 +1717,7 @@
       </c>
       <c r="C20" s="39">
         <f>C5/C6</f>
-        <v>2.8699385697067941</v>
+        <v>1.1359745482432957</v>
       </c>
       <c r="D20" s="39">
         <f>D5/D6</f>
@@ -1666,7 +1725,7 @@
       </c>
       <c r="E20" s="39">
         <f>E5/E6</f>
-        <v>1.7226040825394728</v>
+        <v>2.2817546693407231</v>
       </c>
       <c r="F20" s="39"/>
       <c r="G20" s="39"/>
@@ -1710,19 +1769,19 @@
       </c>
       <c r="B22" s="42">
         <f>B19^2*B18/B13</f>
-        <v>1228.751757325228</v>
+        <v>1295.6612746831017</v>
       </c>
       <c r="C22" s="42">
         <f>C19^2*C18/C13</f>
-        <v>1228.751757325228</v>
+        <v>3239.1531867077547</v>
       </c>
       <c r="D22" s="42">
         <f>D19^2*D18/D13</f>
-        <v>105.3284344470014</v>
+        <v>103.56731594348882</v>
       </c>
       <c r="E22" s="42">
         <f>E19^2*E18/E13</f>
-        <v>105.3284344470014</v>
+        <v>30.786954798896804</v>
       </c>
       <c r="F22" s="42"/>
       <c r="G22" s="42"/>
@@ -1739,19 +1798,19 @@
       </c>
       <c r="B23" s="42">
         <f>B19*12.4*3600/PI()</f>
-        <v>15630.288651168859</v>
+        <v>17051.223983093299</v>
       </c>
       <c r="C23" s="42">
         <f>C19*12.4*3600/PI()</f>
-        <v>15630.288651168859</v>
+        <v>17051.223983093299</v>
       </c>
       <c r="D23" s="42">
         <f>D19*12.4*3600/PI()</f>
-        <v>4262.8059957733249</v>
+        <v>4120.7124625808801</v>
       </c>
       <c r="E23" s="42">
         <f>E19*12.4*3600/PI()</f>
-        <v>4262.8059957733249</v>
+        <v>1420.9353319244419</v>
       </c>
       <c r="F23" s="42"/>
       <c r="G23" s="42"/>
@@ -1768,19 +1827,19 @@
       </c>
       <c r="B24" s="79">
         <f>B22*B17/B23</f>
-        <v>1316.7761897767923</v>
+        <v>1272.7723459887884</v>
       </c>
       <c r="C24" s="79">
         <f>C22*C17/C23</f>
-        <v>1316.7761897767923</v>
+        <v>3181.9308649719715</v>
       </c>
       <c r="D24" s="79">
         <f>D22*D17/D23</f>
-        <v>140.8396434046474</v>
+        <v>143.26010519747575</v>
       </c>
       <c r="E24" s="79">
         <f>E22*E17/E23</f>
-        <v>140.8396434046474</v>
+        <v>123.5000906874791</v>
       </c>
       <c r="F24" s="79"/>
       <c r="G24" s="79"/>
@@ -1800,14 +1859,14 @@
       </c>
       <c r="C25" s="77">
         <f>C22*C7/2*C8/C23</f>
-        <v>1572.2700773454237</v>
+        <v>3799.3204357874292</v>
       </c>
       <c r="D25" s="76" t="s">
         <v>6</v>
       </c>
       <c r="E25" s="77">
         <f>E22*E7/2*E8/E23</f>
-        <v>395.33934990778221</v>
+        <v>346.66692122801152</v>
       </c>
       <c r="F25" s="43"/>
       <c r="G25" s="43"/>
@@ -1827,14 +1886,14 @@
       </c>
       <c r="C26" s="77">
         <f>C19^2*C20/C13*C7/2*C8/C23</f>
-        <v>1481.1522878628059</v>
+        <v>1598.9109746532804</v>
       </c>
       <c r="D26" s="76" t="s">
         <v>6</v>
       </c>
       <c r="E26" s="77">
         <f>E19^2*E20/E13*E7/2*E8/E23</f>
-        <v>193.96847063619333</v>
+        <v>214.10823496102225</v>
       </c>
       <c r="F26" s="43"/>
       <c r="G26" s="43"/>
@@ -1881,14 +1940,14 @@
       </c>
       <c r="C28" s="44">
         <f>C27^2*C20/C13*C9</f>
-        <v>1.5538574582377387</v>
+        <v>1.5376135074699755</v>
       </c>
       <c r="D28" s="40" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="44">
         <f>E27^2*E20/E13*E9</f>
-        <v>0.55459688776460658</v>
+        <v>1.8365422024212092</v>
       </c>
       <c r="F28" s="40"/>
       <c r="G28" s="40"/>
@@ -1908,14 +1967,14 @@
       </c>
       <c r="C29" s="81">
         <f>C28*C7/2*C8/C21</f>
-        <v>76.745327137221338</v>
+        <v>75.943035196564978</v>
       </c>
       <c r="D29" s="80" t="s">
         <v>6</v>
       </c>
       <c r="E29" s="81">
         <f>E28*E7/2*E8/E21</f>
-        <v>28.417213490722222</v>
+        <v>94.1033262218305</v>
       </c>
       <c r="F29" s="82"/>
       <c r="G29" s="82"/>
@@ -2022,19 +2081,19 @@
       <c r="A43" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="B43" s="102">
+      <c r="B43" s="100">
         <f>B6/B8</f>
         <v>1617.3938000000001</v>
       </c>
-      <c r="C43" s="102">
+      <c r="C43" s="100">
         <f t="shared" ref="C43:E43" si="0">C6/C8</f>
         <v>809.87729999999999</v>
       </c>
-      <c r="D43" s="102">
+      <c r="D43" s="100">
         <f t="shared" si="0"/>
         <v>639.30862500000001</v>
       </c>
-      <c r="E43" s="102">
+      <c r="E43" s="100">
         <f t="shared" si="0"/>
         <v>624.51937499999997</v>
       </c>
@@ -2065,7 +2124,7 @@
       <c r="O44" s="57"/>
     </row>
     <row r="45" spans="1:17" s="58" customFormat="1" ht="87.5" x14ac:dyDescent="0.3">
-      <c r="A45" s="98" t="s">
+      <c r="A45" s="97" t="s">
         <v>10</v>
       </c>
       <c r="B45" s="60" t="s">
@@ -2294,7 +2353,7 @@
       <c r="A59" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="B59" s="97">
+      <c r="B59" s="96">
         <v>0.15</v>
       </c>
       <c r="C59" s="49"/>
@@ -2303,7 +2362,7 @@
       <c r="A60" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="B60" s="97">
+      <c r="B60" s="96">
         <v>18.600000000000001</v>
       </c>
       <c r="C60" s="49"/>
@@ -2312,7 +2371,7 @@
       <c r="A61" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="B61" s="97">
+      <c r="B61" s="96">
         <v>12.2</v>
       </c>
       <c r="C61" s="49"/>
@@ -2338,18 +2397,22 @@
         <v>84</v>
       </c>
       <c r="B64" s="32">
-        <v>0.04</v>
-      </c>
-      <c r="C64" s="49"/>
+        <v>0.08</v>
+      </c>
+      <c r="C64" s="111" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="46" t="s">
         <v>85</v>
       </c>
       <c r="B65" s="32">
-        <v>0.04</v>
-      </c>
-      <c r="C65" s="49"/>
+        <v>0.08</v>
+      </c>
+      <c r="C65" s="49" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="46" t="s">
@@ -2358,7 +2421,9 @@
       <c r="B66" s="32">
         <v>9000</v>
       </c>
-      <c r="C66" s="49"/>
+      <c r="C66" s="49" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="46" t="s">
@@ -2367,7 +2432,9 @@
       <c r="B67" s="32">
         <v>10</v>
       </c>
-      <c r="C67" s="49"/>
+      <c r="C67" s="49" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="46" t="s">
@@ -2376,7 +2443,9 @@
       <c r="B68" s="32">
         <v>10</v>
       </c>
-      <c r="C68" s="49"/>
+      <c r="C68" s="49" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="64" t="s">
@@ -2438,16 +2507,20 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="55" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:V80"/>
+  <dimension ref="A1:V186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="G28" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="M181" sqref="M181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2500,22 +2573,22 @@
       <c r="A3" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="101" t="s">
+      <c r="B3" s="112" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101" t="s">
+      <c r="C3" s="112"/>
+      <c r="D3" s="112" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101" t="s">
+      <c r="E3" s="112"/>
+      <c r="F3" s="112" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101" t="s">
+      <c r="G3" s="112"/>
+      <c r="H3" s="112" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="101"/>
+      <c r="I3" s="112"/>
     </row>
     <row r="4" spans="1:22" s="85" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="94"/>
@@ -2642,11 +2715,11 @@
         <v>420000</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="14" x14ac:dyDescent="0.3">
       <c r="A11" s="93">
         <v>1931</v>
       </c>
-      <c r="D11" s="87">
+      <c r="D11" s="101">
         <v>965050</v>
       </c>
       <c r="E11" s="90">
@@ -2764,11 +2837,11 @@
       <c r="T17" s="9"/>
       <c r="U17" s="9"/>
     </row>
-    <row r="18" spans="1:21" ht="13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" ht="14" x14ac:dyDescent="0.3">
       <c r="A18" s="93">
         <v>1938</v>
       </c>
-      <c r="D18" s="96">
+      <c r="D18" s="101">
         <v>920000</v>
       </c>
       <c r="E18" s="90">
@@ -3066,7 +3139,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="14" x14ac:dyDescent="0.3">
       <c r="A45" s="93">
         <v>1965</v>
       </c>
@@ -3076,7 +3149,7 @@
       <c r="C45" s="90">
         <v>48739</v>
       </c>
-      <c r="D45" s="87">
+      <c r="D45" s="101">
         <v>7636675</v>
       </c>
       <c r="E45" s="90">
@@ -3119,11 +3192,11 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A49" s="93">
         <v>1969</v>
       </c>
-      <c r="D49" s="95">
+      <c r="D49" s="102">
         <v>780000</v>
       </c>
     </row>
@@ -3327,11 +3400,11 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A75" s="93">
         <v>1995</v>
       </c>
-      <c r="D75" s="87">
+      <c r="D75" s="101">
         <v>3280000</v>
       </c>
       <c r="E75" s="90">
@@ -3354,11 +3427,11 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A78" s="93">
         <v>1998</v>
       </c>
-      <c r="D78" s="87">
+      <c r="D78" s="101">
         <v>2280000</v>
       </c>
       <c r="E78" s="90">
@@ -3373,12 +3446,932 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A80" s="93">
         <v>2000</v>
       </c>
-      <c r="D80" s="95">
-        <v>280000</v>
+      <c r="D80" s="102">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A81" s="93">
+        <v>2001</v>
+      </c>
+      <c r="D81" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A82" s="93">
+        <v>2002</v>
+      </c>
+      <c r="D82" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A83" s="93">
+        <v>2003</v>
+      </c>
+      <c r="D83" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A84" s="93">
+        <v>2004</v>
+      </c>
+      <c r="D84" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A85" s="93">
+        <v>2005</v>
+      </c>
+      <c r="D85" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A86" s="93">
+        <v>2006</v>
+      </c>
+      <c r="D86" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A87" s="93">
+        <v>2007</v>
+      </c>
+      <c r="D87" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A88" s="93">
+        <v>2008</v>
+      </c>
+      <c r="D88" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A89" s="93">
+        <v>2009</v>
+      </c>
+      <c r="D89" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A90" s="93">
+        <v>2010</v>
+      </c>
+      <c r="D90" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A91" s="93">
+        <v>2011</v>
+      </c>
+      <c r="D91" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A92" s="93">
+        <v>2012</v>
+      </c>
+      <c r="D92" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A93" s="93">
+        <v>2013</v>
+      </c>
+      <c r="D93" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A94" s="93">
+        <v>2014</v>
+      </c>
+      <c r="D94" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A95" s="93">
+        <v>2015</v>
+      </c>
+      <c r="D95" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A96" s="93">
+        <v>2016</v>
+      </c>
+      <c r="D96" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A97" s="93">
+        <v>2017</v>
+      </c>
+      <c r="D97" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A98" s="93">
+        <v>2018</v>
+      </c>
+      <c r="D98" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A99" s="93">
+        <v>2019</v>
+      </c>
+      <c r="D99" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A100" s="93">
+        <v>2020</v>
+      </c>
+      <c r="D100" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A101" s="93">
+        <v>2021</v>
+      </c>
+      <c r="D101" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A102" s="93">
+        <v>2022</v>
+      </c>
+      <c r="D102" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A103" s="93">
+        <v>2023</v>
+      </c>
+      <c r="D103" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A104" s="93">
+        <v>2024</v>
+      </c>
+      <c r="D104" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A105" s="93">
+        <v>2025</v>
+      </c>
+      <c r="D105" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A106" s="93">
+        <v>2026</v>
+      </c>
+      <c r="D106" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A107" s="93">
+        <v>2027</v>
+      </c>
+      <c r="D107" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A108" s="93">
+        <v>2028</v>
+      </c>
+      <c r="D108" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A109" s="93">
+        <v>2029</v>
+      </c>
+      <c r="D109" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A110" s="93">
+        <v>2030</v>
+      </c>
+      <c r="D110" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A111" s="93">
+        <v>2031</v>
+      </c>
+      <c r="D111" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A112" s="93">
+        <v>2032</v>
+      </c>
+      <c r="D112" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A113" s="93">
+        <v>2033</v>
+      </c>
+      <c r="D113" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A114" s="93">
+        <v>2034</v>
+      </c>
+      <c r="D114" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A115" s="93">
+        <v>2035</v>
+      </c>
+      <c r="D115" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A116" s="93">
+        <v>2036</v>
+      </c>
+      <c r="D116" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A117" s="93">
+        <v>2037</v>
+      </c>
+      <c r="D117" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A118" s="93">
+        <v>2038</v>
+      </c>
+      <c r="D118" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A119" s="93">
+        <v>2039</v>
+      </c>
+      <c r="D119" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A120" s="93">
+        <v>2040</v>
+      </c>
+      <c r="D120" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A121" s="93">
+        <v>2041</v>
+      </c>
+      <c r="D121" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A122" s="93">
+        <v>2042</v>
+      </c>
+      <c r="D122" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A123" s="93">
+        <v>2043</v>
+      </c>
+      <c r="D123" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A124" s="93">
+        <v>2044</v>
+      </c>
+      <c r="D124" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A125" s="93">
+        <v>2045</v>
+      </c>
+      <c r="D125" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A126" s="93">
+        <v>2046</v>
+      </c>
+      <c r="D126" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A127" s="93">
+        <v>2047</v>
+      </c>
+      <c r="D127" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A128" s="93">
+        <v>2048</v>
+      </c>
+      <c r="D128" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A129" s="93">
+        <v>2049</v>
+      </c>
+      <c r="D129" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A130" s="93">
+        <v>2050</v>
+      </c>
+      <c r="D130" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A131" s="93">
+        <v>2051</v>
+      </c>
+      <c r="D131" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A132" s="93">
+        <v>2052</v>
+      </c>
+      <c r="D132" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A133" s="93">
+        <v>2053</v>
+      </c>
+      <c r="D133" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A134" s="93">
+        <v>2054</v>
+      </c>
+      <c r="D134" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A135" s="93">
+        <v>2055</v>
+      </c>
+      <c r="D135" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A136" s="93">
+        <v>2056</v>
+      </c>
+      <c r="D136" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A137" s="93">
+        <v>2057</v>
+      </c>
+      <c r="D137" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A138" s="93">
+        <v>2058</v>
+      </c>
+      <c r="D138" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A139" s="93">
+        <v>2059</v>
+      </c>
+      <c r="D139" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A140" s="93">
+        <v>2060</v>
+      </c>
+      <c r="D140" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A141" s="93">
+        <v>2061</v>
+      </c>
+      <c r="D141" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A142" s="93">
+        <v>2062</v>
+      </c>
+      <c r="D142" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A143" s="93">
+        <v>2063</v>
+      </c>
+      <c r="D143" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A144" s="93">
+        <v>2064</v>
+      </c>
+      <c r="D144" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A145" s="93">
+        <v>2065</v>
+      </c>
+      <c r="D145" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A146" s="93">
+        <v>2066</v>
+      </c>
+      <c r="D146" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A147" s="93">
+        <v>2067</v>
+      </c>
+      <c r="D147" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A148" s="93">
+        <v>2068</v>
+      </c>
+      <c r="D148" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A149" s="93">
+        <v>2069</v>
+      </c>
+      <c r="D149" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A150" s="93">
+        <v>2070</v>
+      </c>
+      <c r="D150" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A151" s="93">
+        <v>2071</v>
+      </c>
+      <c r="D151" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A152" s="93">
+        <v>2072</v>
+      </c>
+      <c r="D152" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A153" s="93">
+        <v>2073</v>
+      </c>
+      <c r="D153" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A154" s="93">
+        <v>2074</v>
+      </c>
+      <c r="D154" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A155" s="93">
+        <v>2075</v>
+      </c>
+      <c r="D155" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A156" s="93">
+        <v>2076</v>
+      </c>
+      <c r="D156" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A157" s="93">
+        <v>2077</v>
+      </c>
+      <c r="D157" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A158" s="93">
+        <v>2078</v>
+      </c>
+      <c r="D158" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A159" s="93">
+        <v>2079</v>
+      </c>
+      <c r="D159" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A160" s="93">
+        <v>2080</v>
+      </c>
+      <c r="D160" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A161" s="93">
+        <v>2081</v>
+      </c>
+      <c r="D161" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A162" s="93">
+        <v>2082</v>
+      </c>
+      <c r="D162" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A163" s="93">
+        <v>2083</v>
+      </c>
+      <c r="D163" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A164" s="93">
+        <v>2084</v>
+      </c>
+      <c r="D164" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A165" s="93">
+        <v>2085</v>
+      </c>
+      <c r="D165" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A166" s="93">
+        <v>2086</v>
+      </c>
+      <c r="D166" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A167" s="93">
+        <v>2087</v>
+      </c>
+      <c r="D167" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A168" s="93">
+        <v>2088</v>
+      </c>
+      <c r="D168" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A169" s="93">
+        <v>2089</v>
+      </c>
+      <c r="D169" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A170" s="93">
+        <v>2090</v>
+      </c>
+      <c r="D170" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A171" s="93">
+        <v>2091</v>
+      </c>
+      <c r="D171" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A172" s="93">
+        <v>2092</v>
+      </c>
+      <c r="D172" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A173" s="93">
+        <v>2093</v>
+      </c>
+      <c r="D173" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A174" s="93">
+        <v>2094</v>
+      </c>
+      <c r="D174" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A175" s="93">
+        <v>2095</v>
+      </c>
+      <c r="D175" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A176" s="93">
+        <v>2096</v>
+      </c>
+      <c r="D176" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A177" s="93">
+        <v>2097</v>
+      </c>
+      <c r="D177" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A178" s="93">
+        <v>2098</v>
+      </c>
+      <c r="D178" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A179" s="93">
+        <v>2099</v>
+      </c>
+      <c r="D179" s="95">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A180" s="93">
+        <v>2100</v>
+      </c>
+      <c r="D180" s="95">
+        <v>280000</v>
+      </c>
+      <c r="H180" s="103"/>
+      <c r="I180" s="104"/>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A182" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B182" s="105">
+        <f>Inputs!B5</f>
+        <v>17640829</v>
+      </c>
+      <c r="C182" s="106">
+        <f>Inputs!B6</f>
+        <v>16173938</v>
+      </c>
+      <c r="D182" s="105">
+        <f>Inputs!D5</f>
+        <v>12195117</v>
+      </c>
+      <c r="E182" s="106">
+        <f>Inputs!D6</f>
+        <v>5114469</v>
+      </c>
+      <c r="F182" s="105">
+        <f>Inputs!C5</f>
+        <v>9200000</v>
+      </c>
+      <c r="G182" s="106">
+        <f>Inputs!C6</f>
+        <v>8098773</v>
+      </c>
+      <c r="H182" s="105">
+        <f>Inputs!E5</f>
+        <v>11400000</v>
+      </c>
+      <c r="I182" s="106">
+        <f>Inputs!E6</f>
+        <v>4996155</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A183" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B183" s="105">
+        <f t="shared" ref="B183:I183" si="0">B182+SUM(B6:B180)</f>
+        <v>17685335</v>
+      </c>
+      <c r="C183" s="106">
+        <f t="shared" si="0"/>
+        <v>16222677</v>
+      </c>
+      <c r="D183" s="105">
+        <f t="shared" si="0"/>
+        <v>77406842</v>
+      </c>
+      <c r="E183" s="106">
+        <f t="shared" si="0"/>
+        <v>6168457</v>
+      </c>
+      <c r="F183" s="105">
+        <f t="shared" si="0"/>
+        <v>6504904</v>
+      </c>
+      <c r="G183" s="106">
+        <f t="shared" si="0"/>
+        <v>6237238</v>
+      </c>
+      <c r="H183" s="105">
+        <f t="shared" si="0"/>
+        <v>3062108</v>
+      </c>
+      <c r="I183" s="106">
+        <f t="shared" si="0"/>
+        <v>1397395</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A185" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B185" s="107">
+        <f>B182/C182</f>
+        <v>1.0906947337129647</v>
+      </c>
+      <c r="D185" s="107">
+        <f>D182/E182</f>
+        <v>2.3844346304572381</v>
+      </c>
+      <c r="F185" s="107">
+        <f>F182/G182</f>
+        <v>1.1359745482432957</v>
+      </c>
+      <c r="G185" s="108"/>
+      <c r="H185" s="107">
+        <f>H182/I182</f>
+        <v>2.2817546693407231</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A186" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B186" s="107">
+        <f>B183/C183</f>
+        <v>1.0901613217103441</v>
+      </c>
+      <c r="D186" s="107">
+        <f>D183/E183</f>
+        <v>12.548817637863083</v>
+      </c>
+      <c r="F186" s="107">
+        <f>F183/G183</f>
+        <v>1.0429141873374079</v>
+      </c>
+      <c r="G186" s="108"/>
+      <c r="H186" s="107">
+        <f>H183/I183</f>
+        <v>2.1912973783361185</v>
       </c>
     </row>
   </sheetData>
@@ -3399,8 +4392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C176"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G169" sqref="G169"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3471,11 +4464,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1931</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="109">
         <v>965050</v>
       </c>
       <c r="C7">
@@ -3548,11 +4541,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1938</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="109">
         <v>920000</v>
       </c>
       <c r="C14">
@@ -3889,11 +4882,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="14" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1969</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="109">
         <v>780000</v>
       </c>
       <c r="C45">
@@ -4175,11 +5168,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="14" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>1995</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="109">
         <v>3280000</v>
       </c>
       <c r="C71">
@@ -4208,11 +5201,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="14" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>1998</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="109">
         <v>2280000</v>
       </c>
       <c r="C74">
@@ -5348,10 +6341,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5458,7 +6451,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="30">
-        <v>23242981</v>
+        <v>9200000</v>
       </c>
       <c r="C4" s="30">
         <v>8098773</v>
@@ -5467,7 +6460,7 @@
         <v>10000</v>
       </c>
       <c r="E4">
-        <v>3.0000000000000001E-3</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -5487,7 +6480,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="30">
-        <v>8606397</v>
+        <v>11400000</v>
       </c>
       <c r="C5" s="30">
         <v>4996155</v>
@@ -5496,7 +6489,7 @@
         <v>8000</v>
       </c>
       <c r="E5">
-        <v>3.0000000000000001E-3</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="F5">
         <v>5</v>
@@ -5510,6 +6503,38 @@
       <c r="I5">
         <v>1</v>
       </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>